<commit_message>
modify dtr report dev、buyplan
</commit_message>
<xml_diff>
--- a/DKS-API/Resources/Template/TempDevDtrFgtResultReport_BuyPlan.xlsx
+++ b/DKS-API/Resources/Template/TempDevDtrFgtResultReport_BuyPlan.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>&amp;=result.Article</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -165,6 +165,22 @@
   </si>
   <si>
     <t>&amp;=result.CwaDate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Factory</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Buy Plan Season</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result.Factory</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result.BuyPlanSeason</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -547,149 +563,163 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20" style="6" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" customWidth="1"/>
-    <col min="12" max="12" width="26.28515625" customWidth="1"/>
-    <col min="13" max="13" width="54.140625" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" customWidth="1"/>
-    <col min="15" max="15" width="23" customWidth="1"/>
-    <col min="16" max="16" width="22.7109375" customWidth="1"/>
-    <col min="17" max="17" width="20.42578125" style="6" customWidth="1"/>
-    <col min="18" max="18" width="20.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="6" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" customWidth="1"/>
+    <col min="14" max="14" width="26.28515625" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" customWidth="1"/>
+    <col min="16" max="16" width="23" customWidth="1"/>
+    <col min="17" max="17" width="22.7109375" customWidth="1"/>
+    <col min="18" max="18" width="20.42578125" style="6" customWidth="1"/>
+    <col min="19" max="19" width="20.42578125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="54.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="2" spans="1:18" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R1"/>
+  <autoFilter ref="A1:T1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>